<commit_message>
fixed typo in template, included xml2 package to enable xml download
</commit_message>
<xml_diff>
--- a/PRP_QUANT_V2_itemtypes_sheet_17.xlsx
+++ b/PRP_QUANT_V2_itemtypes_sheet_17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mueller_admin.ZPIDNB21\Documents\Desktop\Rprojects\PRP-QUANT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E982596-B719-40F6-A0C1-5A862D4CD914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F466C0-362E-4084-A476-114270E58A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{74259089-353E-4943-B28F-F01CFF5DD15F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{74259089-353E-4943-B28F-F01CFF5DD15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Titlepage" sheetId="1" r:id="rId1"/>
@@ -582,10 +582,6 @@
   </si>
   <si>
     <t xml:space="preserve">Doing a pilot study is often a good idea! You can upload the description and results of your pilot study separately (select the "Data" collection in PsychArchives or whatever best suits the type of material you are uploading) or as an additional file (PDF/A, csv, code) along with your study protocol.   </t>
-  </si>
-  <si>
-    <t>Sample size is a critical factor in determining statistical power, especially in designs that test against a null hypothesis.  If your statistical power is low, you may fail to detect an existing effect, or you may detect an effect that is not real. Daniel Lakens provides a good overview of different approaches to justifying sample sizes.
-sample size in this article: https://doi.org/10.1525/collabra.33267</t>
   </si>
   <si>
     <t>This item is designed to get you thinking about the characteristics of your sample, e.g., will your participants be WEIRD (White, Educated, Industrialized, Rich, Democratic) and will this likely affect the external validity of your study?</t>
@@ -1270,6 +1266,9 @@
   </si>
   <si>
     <t xml:space="preserve">Even if you are not yet testing specific hypotheses, you can benefit from preregistering the core components of the exploratory parts of your study. </t>
+  </si>
+  <si>
+    <t>Sample size is a critical factor in determining statistical power, especially in designs that test against a null hypothesis.  If your statistical power is low, you may fail to detect an existing effect, or you may detect an effect that is not real. Daniel Lakens provides an excellent overview of different approaches to justifying sample size in this article: https://doi.org/10.1525/collabra.33267</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1779,7 @@
         <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1809,7 +1808,7 @@
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L4" t="s">
         <v>49</v>
@@ -1832,7 +1831,7 @@
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J5" t="s">
         <v>39</v>
@@ -1984,7 +1983,7 @@
         <v>102</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2045,7 +2044,7 @@
         <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2170,7 +2169,7 @@
         <v>107</v>
       </c>
       <c r="L8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2248,7 +2247,7 @@
         <v>85</v>
       </c>
       <c r="I11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J11" t="s">
         <v>57</v>
@@ -2268,13 +2267,13 @@
         <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I12" t="s">
         <v>99</v>
@@ -2320,7 +2319,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -2434,7 +2433,7 @@
         <v>127</v>
       </c>
       <c r="K3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L3" t="s">
         <v>120</v>
@@ -2510,13 +2509,13 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J2" t="s">
         <v>128</v>
       </c>
       <c r="K2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L2" t="s">
         <v>140</v>
@@ -2542,7 +2541,7 @@
         <v>129</v>
       </c>
       <c r="K3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L3" t="s">
         <v>141</v>
@@ -2556,13 +2555,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J4" t="s">
         <v>130</v>
@@ -2582,7 +2581,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -2597,7 +2596,7 @@
         <v>131</v>
       </c>
       <c r="K5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2644,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72AF7E5-B12E-4B8F-A8D9-D3092477F96D}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,7 +2709,7 @@
         <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J2" t="s">
         <v>148</v>
@@ -2742,13 +2741,13 @@
         <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J3" t="s">
         <v>148</v>
       </c>
       <c r="K3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L3" t="s">
         <v>169</v>
@@ -2768,7 +2767,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J4" t="s">
         <v>149</v>
@@ -2791,13 +2790,13 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J5" t="s">
         <v>150</v>
       </c>
       <c r="K5" t="s">
-        <v>175</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
@@ -2814,13 +2813,13 @@
         <v>20</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J6" t="s">
         <v>151</v>
       </c>
       <c r="K6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L6" t="s">
         <v>170</v>
@@ -2840,13 +2839,13 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J7" t="s">
         <v>152</v>
       </c>
       <c r="K7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L7" t="s">
         <v>171</v>
@@ -2866,13 +2865,13 @@
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J8" t="s">
         <v>153</v>
       </c>
       <c r="K8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L8" t="s">
         <v>172</v>
@@ -2886,19 +2885,19 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J9" t="s">
         <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2956,91 +2955,91 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
+        <v>271</v>
+      </c>
+      <c r="I4" t="s">
         <v>272</v>
       </c>
-      <c r="I4" t="s">
-        <v>273</v>
-      </c>
       <c r="J4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>296</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>297</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3049,88 +3048,88 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J8" t="s">
         <v>59</v>
       </c>
       <c r="K8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3142,7 +3141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8B6A50-F72F-4DEF-908B-E1599CB4BCD6}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -3191,91 +3190,91 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3284,197 +3283,197 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -3489,36 +3488,36 @@
         <v>85</v>
       </c>
       <c r="I13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
       <c r="I14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3576,45 +3575,45 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K3" t="s">
         <v>47</v>

</xml_diff>